<commit_message>
added char stats list, started stats generation
</commit_message>
<xml_diff>
--- a/Предметы.xlsx
+++ b/Предметы.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Chest Clicker RPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A9C9C8-FE6A-4D30-8A84-BC736AEAC705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AE7A35-039D-4781-87B1-02A929B92FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28575" yWindow="1740" windowWidth="23040" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="3036" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Редкость" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="126">
   <si>
     <t>Эпический</t>
   </si>
@@ -373,18 +381,175 @@
   </si>
   <si>
     <t>Аксессуар</t>
+  </si>
+  <si>
+    <t>Героический</t>
+  </si>
+  <si>
+    <t>Легендарный</t>
+  </si>
+  <si>
+    <t>предметы</t>
+  </si>
+  <si>
+    <t>свойства</t>
+  </si>
+  <si>
+    <t>6 + 2 онли дроп</t>
+  </si>
+  <si>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>2+1</t>
+  </si>
+  <si>
+    <t>3+1</t>
+  </si>
+  <si>
+    <t>4+1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -413,8 +578,17 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +691,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF301"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE60000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -582,21 +768,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -672,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -690,6 +876,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -698,6 +890,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE60000"/>
+      <color rgb="FFFFF301"/>
       <color rgb="FFFF6600"/>
       <color rgb="FF33CC33"/>
       <color rgb="FF00FF00"/>
@@ -706,7 +900,6 @@
       <color rgb="FF26EB07"/>
       <color rgb="FF017A07"/>
       <color rgb="FF0ED44B"/>
-      <color rgb="FF14F058"/>
     </mruColors>
   </colors>
   <extLst>
@@ -984,23 +1177,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A3:J18"/>
+  <dimension ref="A3:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.5546875" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -1147,7 +1341,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1155,12 +1349,66 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="I22" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" s="41" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>